<commit_message>
sch update layout update
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec.xlsx
+++ b/1-SystemDocs/System_spec.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="13" r:id="rId1"/>
@@ -1408,7 +1408,7 @@
         <xdr:cNvPr id="2" name="Obrázok 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1745,8 +1745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1881,7 +1881,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,11 +2039,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="53" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -2148,8 +2149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3271,7 +3272,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3687,8 +3688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B22:H58"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
SD and ethernet merged
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec.xlsx
+++ b/1-SystemDocs/System_spec.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="7" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="13" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="TO DO" sheetId="8" r:id="rId11"/>
     <sheet name="System setup" sheetId="12" r:id="rId12"/>
     <sheet name="Sensors Example datasheet val." sheetId="14" r:id="rId13"/>
+    <sheet name="IssueTracking" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="294">
   <si>
     <t>ETH*</t>
   </si>
@@ -906,6 +907,24 @@
   </si>
   <si>
     <t>find alternative</t>
+  </si>
+  <si>
+    <t>change SHCP timeout from 1s back to 60s</t>
+  </si>
+  <si>
+    <t>SD status flag to UDP</t>
+  </si>
+  <si>
+    <t>IssueTracking!A1</t>
+  </si>
+  <si>
+    <t>add I2C address selecting resistors in case some sensor has conflicting address</t>
+  </si>
+  <si>
+    <t>IO expander, add 0R to A2 input to VCC and GND. This will enable using PCA9539 too</t>
+  </si>
+  <si>
+    <t>NXP datasheet: The PCA9539; PCA9539R is identical to the PCA9555 except for the removal of the internal I/O pull-up resistor which greatly reduces power consumption when the I/Os are held LOW, replacement of A2 with RESET and a different address range</t>
   </si>
 </sst>
 </file>
@@ -1745,7 +1764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1818,7 +1837,9 @@
       </c>
     </row>
     <row r="14" spans="2:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="B14" s="56"/>
+      <c r="B14" s="56" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="15" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B15" s="56"/>
@@ -1870,9 +1891,10 @@
     <hyperlink ref="B11" location="'TO DO'!A1" display="'TO DO'!A1"/>
     <hyperlink ref="B12" location="'System setup'!A1" display="'System setup'!A1"/>
     <hyperlink ref="B13" location="'Sensors Example datasheet val.'!A1" display="'Sensors Example datasheet val.'!A1"/>
+    <hyperlink ref="B14" location="IssueTracking!A1" display="IssueTracking!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1998,10 +2020,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,6 +2050,16 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -2149,9 +2181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2521,12 +2551,51 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="83.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="58" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Contents!A1" display="Contents!A1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="B1" sqref="B1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
announcements, io expander, ...
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec.xlsx
+++ b/1-SystemDocs/System_spec.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="7" activeTab="13"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="13" r:id="rId1"/>
@@ -20,13 +20,17 @@
     <sheet name="UDP packets" sheetId="5" r:id="rId6"/>
     <sheet name="UDP datagram definition" sheetId="6" r:id="rId7"/>
     <sheet name="Message Types" sheetId="7" r:id="rId8"/>
-    <sheet name="ADC selection" sheetId="9" r:id="rId9"/>
-    <sheet name="Time budget" sheetId="11" r:id="rId10"/>
-    <sheet name="TO DO" sheetId="8" r:id="rId11"/>
-    <sheet name="System setup" sheetId="12" r:id="rId12"/>
-    <sheet name="Sensors Example datasheet val." sheetId="14" r:id="rId13"/>
-    <sheet name="IssueTracking" sheetId="15" r:id="rId14"/>
+    <sheet name="Error Codes" sheetId="16" r:id="rId9"/>
+    <sheet name="ADC selection" sheetId="9" r:id="rId10"/>
+    <sheet name="Time budget" sheetId="11" r:id="rId11"/>
+    <sheet name="TO DO" sheetId="8" r:id="rId12"/>
+    <sheet name="System setup" sheetId="12" r:id="rId13"/>
+    <sheet name="Sensors Example datasheet val." sheetId="14" r:id="rId14"/>
+    <sheet name="IssueTracking" sheetId="15" r:id="rId15"/>
   </sheets>
+  <definedNames>
+    <definedName name="error_codes" localSheetId="8">'Error Codes'!$A$4:$B$11</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,8 +46,21 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="error_codes" type="6" refreshedVersion="5" background="1" refreshOnLoad="1" saveData="1">
+    <textPr codePage="850" sourceFile="D:\PROJECTS\01_GIT_REPOS\FRA_Sensor_platform\3-FW_SW\2-SW_log_PC\1-LabVIEW_app\error_codes.csv" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="325">
   <si>
     <t>ETH*</t>
   </si>
@@ -345,9 +362,6 @@
     <t>uint_16</t>
   </si>
   <si>
-    <t>int_32</t>
-  </si>
-  <si>
     <t>Message type</t>
   </si>
   <si>
@@ -357,15 +371,6 @@
     <t>EOP</t>
   </si>
   <si>
-    <t>timestamp epoch time MSB</t>
-  </si>
-  <si>
-    <t>timestamp epoch time</t>
-  </si>
-  <si>
-    <t>timestamp epoch time LSB</t>
-  </si>
-  <si>
     <t>uint_32</t>
   </si>
   <si>
@@ -414,9 +419,6 @@
     <t>ERROR CODE</t>
   </si>
   <si>
-    <t>unknown error</t>
-  </si>
-  <si>
     <t>ERROR</t>
   </si>
   <si>
@@ -570,9 +572,6 @@
     <t>ANNOUNCEMENT announcing sensor unit is on network</t>
   </si>
   <si>
-    <t>COMMAND</t>
-  </si>
-  <si>
     <t>5..8</t>
   </si>
   <si>
@@ -925,13 +924,124 @@
   </si>
   <si>
     <t>NXP datasheet: The PCA9539; PCA9539R is identical to the PCA9555 except for the removal of the internal I/O pull-up resistor which greatly reduces power consumption when the I/Os are held LOW, replacement of A2 with RESET and a different address range</t>
+  </si>
+  <si>
+    <t>ERROR CODES</t>
+  </si>
+  <si>
+    <t>Error Codes'!A1</t>
+  </si>
+  <si>
+    <t>failed to initalize Ethernet controller</t>
+  </si>
+  <si>
+    <t>failed to obtaiin IP from DHCP server</t>
+  </si>
+  <si>
+    <t>SD full card resolution</t>
+  </si>
+  <si>
+    <t>SD card communication fail, continuing with no logging to SD card</t>
+  </si>
+  <si>
+    <t>failed to initalize I2C bus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">failed to initalize IO Expander </t>
+  </si>
+  <si>
+    <t>failed to initalize ADC</t>
+  </si>
+  <si>
+    <t>No error</t>
+  </si>
+  <si>
+    <t>error in setting time. time is from the past. time not set. continuing</t>
+  </si>
+  <si>
+    <t>DO NOT ADD ERROR CODES TO THIS LIST, EDIT SOURCE FILE HERE:</t>
+  </si>
+  <si>
+    <t>D:\PROJECTS\01_GIT_REPOS\FRA_Sensor_platform\3-FW_SW\2-SW_log_PC\1-LabVIEW_app</t>
+  </si>
+  <si>
+    <t>sender number</t>
+  </si>
+  <si>
+    <t>Sensor power control</t>
+  </si>
+  <si>
+    <t>Set period</t>
+  </si>
+  <si>
+    <t>timestamp epoch time or sample order MSB</t>
+  </si>
+  <si>
+    <t>timestamp epoch time or sample order LSB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timestamp epoch time or sample order </t>
+  </si>
+  <si>
+    <t>Sensor unit to Master</t>
+  </si>
+  <si>
+    <t>Master to Sensor unit</t>
+  </si>
+  <si>
+    <t>Command / ACK</t>
+  </si>
+  <si>
+    <t>uint8_t</t>
+  </si>
+  <si>
+    <t>Unit/sender number - last byte of IP</t>
+  </si>
+  <si>
+    <t>0xFFFF</t>
+  </si>
+  <si>
+    <t>Power to all sensors on</t>
+  </si>
+  <si>
+    <t>0x0000</t>
+  </si>
+  <si>
+    <t>Power to all sensors off</t>
+  </si>
+  <si>
+    <t>5..6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: all combinations of bits. Ordered as on IO expander </t>
+  </si>
+  <si>
+    <t>Sensor power report</t>
+  </si>
+  <si>
+    <t>Inverted logic levels on IO expander pins</t>
+  </si>
+  <si>
+    <t>Sensor unit</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>Sensor unit enters IDLE state</t>
+  </si>
+  <si>
+    <t>Master logs error</t>
+  </si>
+  <si>
+    <t>Master checks against requested setting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1021,8 +1131,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1092,6 +1216,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1227,7 +1363,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1329,6 +1465,39 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextové prepojenie" xfId="1" builtinId="8"/>
@@ -1427,7 +1596,7 @@
         <xdr:cNvPr id="2" name="Obrázok 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1457,6 +1626,261 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Rovná spojovacia šípka 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3638550" y="1104900"/>
+          <a:ext cx="1200150" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Rovná spojovacia šípka 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3638550" y="1857375"/>
+          <a:ext cx="1181100" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Rovná spojovacia šípka 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3638550" y="4581525"/>
+          <a:ext cx="1181100" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Rovná spojovacia šípka 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3676650" y="4953000"/>
+          <a:ext cx="1200150" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Rovná spojovacia šípka 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3581400" y="2933700"/>
+          <a:ext cx="1257300" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1497,6 +1921,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="error_codes" refreshOnLoad="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1762,10 +2190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B26"/>
+  <dimension ref="B1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,71 +2206,73 @@
     </row>
     <row r="2" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="56" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="56" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="56" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="56" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="56" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B7" s="56" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="56" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B9" s="56" t="s">
-        <v>208</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="56" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B11" s="56" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="56" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="56" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="56" t="s">
-        <v>290</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="B15" s="56"/>
+      <c r="B15" s="56" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="16" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B16" s="56"/>
@@ -1876,6 +2306,9 @@
     </row>
     <row r="26" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B26" s="56"/>
+    </row>
+    <row r="27" spans="2:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="B27" s="56"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1886,12 +2319,13 @@
     <hyperlink ref="B6" location="'UDP packets'!A1" display="'UDP packets'!A1"/>
     <hyperlink ref="B7" location="'UDP datagram definition'!A1" display="'UDP datagram definition'!A1"/>
     <hyperlink ref="B8" location="'Message Types'!A1" display="'Message Types'!A1"/>
-    <hyperlink ref="B9" location="'ADC selection'!A1" display="'ADC selection'!A1"/>
-    <hyperlink ref="B10" location="'Time budget'!A1" display="'Time budget'!A1"/>
-    <hyperlink ref="B11" location="'TO DO'!A1" display="'TO DO'!A1"/>
-    <hyperlink ref="B12" location="'System setup'!A1" display="'System setup'!A1"/>
-    <hyperlink ref="B13" location="'Sensors Example datasheet val.'!A1" display="'Sensors Example datasheet val.'!A1"/>
-    <hyperlink ref="B14" location="IssueTracking!A1" display="IssueTracking!A1"/>
+    <hyperlink ref="B10" location="'ADC selection'!A1" display="'ADC selection'!A1"/>
+    <hyperlink ref="B11" location="'Time budget'!A1" display="'Time budget'!A1"/>
+    <hyperlink ref="B12" location="'TO DO'!A1" display="'TO DO'!A1"/>
+    <hyperlink ref="B13" location="'System setup'!A1" display="'System setup'!A1"/>
+    <hyperlink ref="B14" location="'Sensors Example datasheet val.'!A1" display="'Sensors Example datasheet val.'!A1"/>
+    <hyperlink ref="B15" location="IssueTracking!A1" display="IssueTracking!A1"/>
+    <hyperlink ref="B9" location="'Error Codes'!A1" display="'Error Codes'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
@@ -1899,6 +2333,113 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -1918,12 +2459,12 @@
         <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1932,12 +2473,12 @@
         <v>284</v>
       </c>
       <c r="I2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -1948,7 +2489,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B4">
         <v>68</v>
@@ -1957,59 +2498,59 @@
         <v>9000</v>
       </c>
       <c r="D4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B9">
         <v>400</v>
       </c>
       <c r="C9" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B10">
         <f>1/(B9)</f>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="C10" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B11">
         <f>B10*16</f>
         <v>0.04</v>
       </c>
       <c r="C11" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B12">
         <f>B11*9</f>
         <v>0.36</v>
       </c>
       <c r="C12" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2018,60 +2559,73 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" t="s">
-        <v>199</v>
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="58" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>288</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>289</v>
+        <v>282</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Contents!A1" display="Contents!A1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2083,7 +2637,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2091,7 +2645,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2099,7 +2653,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2107,7 +2661,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2115,7 +2669,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2123,7 +2677,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2131,7 +2685,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2139,7 +2693,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2177,7 +2731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
@@ -2198,42 +2752,42 @@
   <sheetData>
     <row r="1" spans="1:13" s="59" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="58" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="H2" t="s">
+        <v>211</v>
+      </c>
+      <c r="I2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J2" t="s">
+        <v>213</v>
+      </c>
+      <c r="K2" t="s">
+        <v>270</v>
+      </c>
+      <c r="L2" t="s">
         <v>217</v>
       </c>
-      <c r="I2" t="s">
-        <v>218</v>
-      </c>
-      <c r="J2" t="s">
-        <v>219</v>
-      </c>
-      <c r="K2" t="s">
-        <v>276</v>
-      </c>
-      <c r="L2" t="s">
-        <v>223</v>
-      </c>
       <c r="M2" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2241,34 +2795,34 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F3">
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="H3" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="I3" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="J3" s="60" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="K3" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="L3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2276,28 +2830,28 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F4" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="H4" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="J4" s="61" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="K4" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="L4" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2305,31 +2859,31 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G5" t="s">
+        <v>231</v>
+      </c>
+      <c r="H5" t="s">
+        <v>225</v>
+      </c>
+      <c r="I5" t="s">
+        <v>229</v>
+      </c>
+      <c r="J5" s="62" t="s">
+        <v>232</v>
+      </c>
+      <c r="K5" t="s">
+        <v>273</v>
+      </c>
+      <c r="M5" s="57" t="s">
         <v>234</v>
-      </c>
-      <c r="D5" t="s">
-        <v>236</v>
-      </c>
-      <c r="E5" t="s">
-        <v>242</v>
-      </c>
-      <c r="G5" t="s">
-        <v>237</v>
-      </c>
-      <c r="H5" t="s">
-        <v>231</v>
-      </c>
-      <c r="I5" t="s">
-        <v>235</v>
-      </c>
-      <c r="J5" s="62" t="s">
-        <v>238</v>
-      </c>
-      <c r="K5" t="s">
-        <v>279</v>
-      </c>
-      <c r="M5" s="57" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2337,25 +2891,25 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D6" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="F6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H6" t="s">
         <v>245</v>
       </c>
-      <c r="H6" t="s">
-        <v>251</v>
-      </c>
       <c r="I6" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="J6" s="61" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="K6" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2363,25 +2917,25 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
+        <v>240</v>
+      </c>
+      <c r="D7" t="s">
+        <v>241</v>
+      </c>
+      <c r="F7" t="s">
+        <v>239</v>
+      </c>
+      <c r="H7" t="s">
         <v>246</v>
       </c>
-      <c r="D7" t="s">
-        <v>247</v>
-      </c>
-      <c r="F7" t="s">
-        <v>245</v>
-      </c>
-      <c r="H7" t="s">
-        <v>252</v>
-      </c>
       <c r="I7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="J7" s="61" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="K7" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2389,19 +2943,19 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D8" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="H8" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="I8" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="J8" s="61" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2409,28 +2963,28 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D9" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="F9" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="G9" t="s">
+        <v>251</v>
+      </c>
+      <c r="H9" t="s">
         <v>257</v>
       </c>
-      <c r="H9" t="s">
-        <v>263</v>
-      </c>
       <c r="I9" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="J9" s="64" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="L9" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2438,25 +2992,25 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="D10" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F10" t="s">
         <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="H10" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="I10" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="J10" s="64" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2464,19 +3018,19 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D11" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="H11" t="s">
+        <v>261</v>
+      </c>
+      <c r="I11" t="s">
         <v>267</v>
       </c>
-      <c r="I11" t="s">
-        <v>273</v>
-      </c>
       <c r="J11" s="63" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2484,22 +3038,22 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
+        <v>262</v>
+      </c>
+      <c r="D12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F12" t="s">
+        <v>264</v>
+      </c>
+      <c r="H12" t="s">
+        <v>265</v>
+      </c>
+      <c r="I12" t="s">
+        <v>266</v>
+      </c>
+      <c r="J12" s="65" t="s">
         <v>268</v>
-      </c>
-      <c r="D12" t="s">
-        <v>269</v>
-      </c>
-      <c r="F12" t="s">
-        <v>270</v>
-      </c>
-      <c r="H12" t="s">
-        <v>271</v>
-      </c>
-      <c r="I12" t="s">
-        <v>272</v>
-      </c>
-      <c r="J12" s="65" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2507,10 +3061,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="J13" s="64" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2518,13 +3072,13 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="H14" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="J14" s="66" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2551,13 +3105,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2566,20 +3118,20 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="58" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B4" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -2609,7 +3161,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
@@ -2633,7 +3185,7 @@
         <v>74</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -2716,7 +3268,7 @@
         <v>44</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="L4" s="1">
         <v>4</v>
@@ -2745,10 +3297,10 @@
         <v>12</v>
       </c>
       <c r="J5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="L5" s="1">
         <v>17</v>
@@ -2777,7 +3329,7 @@
         <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>14</v>
@@ -2850,7 +3402,7 @@
         <v>23</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="L9" s="1">
         <v>23</v>
@@ -3458,7 +4010,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3518,18 +4070,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E3" sqref="E3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.140625" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
@@ -3540,313 +4092,503 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="71" t="s">
+        <v>307</v>
+      </c>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="E3" s="71" t="s">
+        <v>308</v>
+      </c>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>96</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>97</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>98</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E4" t="s">
         <v>96</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F4" t="s">
         <v>97</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G4" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
-        <v>0</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="16">
-        <v>0</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
-        <v>1</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4" s="16">
-        <v>1</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>105</v>
+        <v>304</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E5" s="16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
+        <v>1</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="16">
+        <v>1</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>2</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="16">
+        <v>2</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="16" t="s">
+      <c r="B8" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="16">
+        <v>3</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>4</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="16">
-        <v>3</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="G6" s="16" t="s">
+      <c r="C9" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="17">
+        <v>4</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
-        <v>4</v>
-      </c>
-      <c r="B7" s="17" t="s">
+      <c r="G9" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="17">
-        <v>4</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="69">
         <v>5</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9">
+      <c r="B10" s="69" t="s">
+        <v>311</v>
+      </c>
+      <c r="C10" s="69" t="s">
+        <v>310</v>
+      </c>
+      <c r="E10" s="69">
         <v>5</v>
       </c>
-      <c r="G9" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10">
-        <v>6</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>107</v>
+      <c r="F10" s="69" t="s">
+        <v>309</v>
+      </c>
+      <c r="G10" s="69" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="E13">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>11</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E3:G3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B22:H58"/>
+  <dimension ref="B2:J63"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" s="21" t="s">
+    <row r="2" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="71" t="s">
+        <v>320</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="H2" s="71" t="s">
+        <v>321</v>
+      </c>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="22">
+        <v>4</v>
+      </c>
+      <c r="C5" s="18">
+        <v>4</v>
+      </c>
+      <c r="D5" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="F5" s="72"/>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H7" s="22">
+        <v>4</v>
+      </c>
+      <c r="I7" s="18">
+        <v>1</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="J8" s="26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="29"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="30">
+        <v>4</v>
+      </c>
+      <c r="C13" s="31">
+        <v>3</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="H13" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="30">
+        <v>5</v>
+      </c>
+      <c r="C14" s="31" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B24" s="22">
+      <c r="D14" s="37" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="34">
+        <v>6</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="70" t="s">
+        <v>118</v>
+      </c>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H17" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="J17" s="29"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H18" s="30">
         <v>4</v>
       </c>
-      <c r="C24" s="18">
+      <c r="I18" s="31">
+        <v>5</v>
+      </c>
+      <c r="J18" s="37" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H19" s="79" t="s">
+        <v>316</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="J19" s="37" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H20" s="30"/>
+      <c r="I20" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="J20" s="37" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="73" t="s">
+        <v>317</v>
+      </c>
+      <c r="I21" s="74"/>
+      <c r="J21" s="75"/>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="78"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="30">
         <v>4</v>
       </c>
-      <c r="D24" s="55" t="s">
+      <c r="C23" s="31">
+        <v>5</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="30">
+        <v>5</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="80" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="22">
-        <v>4</v>
-      </c>
-      <c r="C28" s="18">
-        <v>1</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="C29" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="D29" s="26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="81" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H30" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="J30" s="29"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="27" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D31" s="29"/>
-      <c r="H31" s="13"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="30"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="32"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="30">
         <v>4</v>
       </c>
@@ -3854,444 +4596,426 @@
         <v>2</v>
       </c>
       <c r="D32" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="H32" s="30"/>
+      <c r="I32" s="31">
+        <v>6</v>
+      </c>
+      <c r="J32" s="32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="H33" s="30"/>
+      <c r="I33" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="J33" s="32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="H34" s="30"/>
+      <c r="I34" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="H32" s="13"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="D33" s="32" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="32" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J34" s="32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="30" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="H35" s="30"/>
+      <c r="I35" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="J35" s="32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="30"/>
       <c r="C36" s="31" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="H36" s="30"/>
+      <c r="I36" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="J36" s="37" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="H37" s="30"/>
+      <c r="I37" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="J37" s="37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H38" s="30"/>
+      <c r="I38" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="J38" s="32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H39" s="30"/>
+      <c r="I39" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="J39" s="32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H40" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="I40" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="J40" s="37" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H41" s="30"/>
+      <c r="I41" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="J41" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H42" s="34"/>
+      <c r="I42" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="J42" s="36" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D46" s="29"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="30">
+        <v>4</v>
+      </c>
+      <c r="C47" s="31">
+        <v>5</v>
+      </c>
+      <c r="D47" s="37" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="33"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="30"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="30"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="30"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="30"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="38"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="30"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="30"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="D37" s="32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="C38" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="D38" s="36" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="C40" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="D40" s="29"/>
-      <c r="F40" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="G40" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="H40" s="29"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="30">
-        <v>4</v>
-      </c>
-      <c r="C41" s="31">
-        <v>3</v>
-      </c>
-      <c r="D41" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="F41" s="30">
-        <v>4</v>
-      </c>
-      <c r="G41" s="31">
-        <v>3</v>
-      </c>
-      <c r="H41" s="32"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="C42" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="D42" s="32"/>
-      <c r="F42" s="30">
-        <v>5</v>
-      </c>
-      <c r="G42" s="31">
-        <v>4</v>
-      </c>
-      <c r="H42" s="32" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="30"/>
-      <c r="C43" s="30">
-        <v>1</v>
-      </c>
-      <c r="D43" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="F43" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="G43" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="H43" s="32" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="30"/>
-      <c r="C44" s="30">
-        <v>2</v>
-      </c>
-      <c r="D44" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="F44" s="34"/>
-      <c r="G44" s="35">
-        <v>1</v>
-      </c>
-      <c r="H44" s="36" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="30"/>
-      <c r="C45" s="30">
-        <v>3</v>
-      </c>
-      <c r="D45" s="32" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="30"/>
-      <c r="C46" s="30">
-        <v>4</v>
-      </c>
-      <c r="D46" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="F46" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="G46" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="H46" s="29"/>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="38"/>
-      <c r="C47" s="38">
-        <v>5</v>
-      </c>
-      <c r="D47" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="F47" s="30">
-        <v>4</v>
-      </c>
-      <c r="G47" s="31">
-        <v>3</v>
-      </c>
-      <c r="H47" s="32"/>
-    </row>
-    <row r="48" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="34"/>
-      <c r="C48" s="34">
-        <v>6</v>
-      </c>
-      <c r="D48" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="F48" s="30">
-        <v>5</v>
-      </c>
-      <c r="G48" s="31">
-        <v>6</v>
-      </c>
-      <c r="H48" s="32" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C49" s="38">
-        <v>7</v>
-      </c>
-      <c r="D49" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="F49" s="30">
-        <v>6</v>
-      </c>
-      <c r="G49" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="H49" s="32" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C50" s="38">
-        <v>8</v>
-      </c>
-      <c r="D50" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="F50" s="30"/>
-      <c r="G50" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="H50" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="F51" s="30">
-        <v>7</v>
-      </c>
-      <c r="G51" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="H51" s="32" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="F52" s="30"/>
-      <c r="G52" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="H52" s="37" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="F53" s="30"/>
-      <c r="G53" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="H53" s="37" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="F54" s="30">
-        <v>8</v>
-      </c>
-      <c r="G54" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="H54" s="32" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="F55" s="30">
-        <v>9</v>
-      </c>
-      <c r="G55" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="H55" s="32" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="F56" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="G56" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="H56" s="37" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="F57" s="30">
-        <v>28</v>
-      </c>
-      <c r="G57" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="H57" s="32" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="58" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F58" s="34">
-        <v>29</v>
-      </c>
-      <c r="G58" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="H58" s="36" t="s">
-        <v>136</v>
-      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="30"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="37" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="30"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="37" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="30"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="32"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="30"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="32"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="30"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="32"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="30"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="32"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="30"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="32"/>
+    </row>
+    <row r="63" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="34"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="36"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H21:J22"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D15" location="'Error Codes'!A1" display="ERROR CODE"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="61.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C1" t="s">
-        <v>146</v>
+    <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="58" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>148</v>
+      <c r="D2" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="67" t="s">
+        <v>288</v>
+      </c>
+      <c r="D3" s="30">
+        <v>4</v>
+      </c>
+      <c r="E3" s="31">
+        <v>3</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>153</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="C4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5" t="s">
-        <v>156</v>
-      </c>
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D4" s="30">
+        <v>5</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" s="68" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="C6" t="s">
-        <v>152</v>
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="C7" t="s">
-        <v>152</v>
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>159</v>
-      </c>
-      <c r="B8" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="C8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>294</v>
+      </c>
+      <c r="D8" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>298</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" location="Contents!A1" display="Contents!A1"/>
+    <hyperlink ref="F4" location="'Error Codes'!A1" display="ERROR CODE"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
power reports done, interrupt ethernet..
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec.xlsx
+++ b/1-SystemDocs/System_spec.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="4" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="13" r:id="rId1"/>
@@ -21,12 +21,13 @@
     <sheet name="UDP datagram definition" sheetId="6" r:id="rId7"/>
     <sheet name="Message Types" sheetId="7" r:id="rId8"/>
     <sheet name="Error Codes" sheetId="16" r:id="rId9"/>
-    <sheet name="ADC selection" sheetId="9" r:id="rId10"/>
-    <sheet name="Time budget" sheetId="11" r:id="rId11"/>
-    <sheet name="TO DO" sheetId="8" r:id="rId12"/>
-    <sheet name="System setup" sheetId="12" r:id="rId13"/>
-    <sheet name="Sensors Example datasheet val." sheetId="14" r:id="rId14"/>
-    <sheet name="IssueTracking" sheetId="15" r:id="rId15"/>
+    <sheet name="LW Error Codes" sheetId="17" r:id="rId10"/>
+    <sheet name="ADC selection" sheetId="9" r:id="rId11"/>
+    <sheet name="Time budget" sheetId="11" r:id="rId12"/>
+    <sheet name="TO DO" sheetId="8" r:id="rId13"/>
+    <sheet name="System setup" sheetId="12" r:id="rId14"/>
+    <sheet name="Sensors Example datasheet val." sheetId="14" r:id="rId15"/>
+    <sheet name="IssueTracking" sheetId="15" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="error_codes" localSheetId="8">'Error Codes'!$A$4:$B$11</definedName>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="343">
   <si>
     <t>ETH*</t>
   </si>
@@ -1013,9 +1014,6 @@
     <t>5..6</t>
   </si>
   <si>
-    <t xml:space="preserve">Note: all combinations of bits. Ordered as on IO expander </t>
-  </si>
-  <si>
     <t>Sensor power report</t>
   </si>
   <si>
@@ -1035,6 +1033,63 @@
   </si>
   <si>
     <t>Master checks against requested setting</t>
+  </si>
+  <si>
+    <t>Labview error codes</t>
+  </si>
+  <si>
+    <t>Power setting not accepted. Invalid input</t>
+  </si>
+  <si>
+    <t>RESET unit</t>
+  </si>
+  <si>
+    <t>IC9 heat pad unmask</t>
+  </si>
+  <si>
+    <t>10k is 1206 - fix in BOM to 0602</t>
+  </si>
+  <si>
+    <t>R46 replace with ferite bead</t>
+  </si>
+  <si>
+    <t>cp2101 edit footprint, corner out</t>
+  </si>
+  <si>
+    <t>remove SD connector</t>
+  </si>
+  <si>
+    <t>rotate microSD connector 180 deg.</t>
+  </si>
+  <si>
+    <t>blocking cap to IO expander?</t>
+  </si>
+  <si>
+    <t>Note: all combinations of bits. Ordered as on IO expander. Log 1 will turn the output of IO exp LOW, thus voltage output on sensor port HIGH. Byte 5 controls port 1, byte 6 is for port 0.</t>
+  </si>
+  <si>
+    <t>Error message not received in some cases</t>
+  </si>
+  <si>
+    <t>R1. R2 10k? Test on 2nd board</t>
+  </si>
+  <si>
+    <t>C10 10u/25V place</t>
+  </si>
+  <si>
+    <t>C17 place 10u 10v normal</t>
+  </si>
+  <si>
+    <t>pca9555 check packageing</t>
+  </si>
+  <si>
+    <t>change pca9555 so also the other one can be used</t>
+  </si>
+  <si>
+    <t>C16 change to 10u, avoid loading fw problems</t>
+  </si>
+  <si>
+    <t>SMPS  inductors  to SRP5030CA-1R5M</t>
   </si>
 </sst>
 </file>
@@ -1469,11 +1524,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1492,11 +1552,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1596,7 +1651,7 @@
         <xdr:cNvPr id="2" name="Obrázok 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2334,6 +2389,67 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="58" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="67" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>500</v>
+      </c>
+      <c r="B4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="68"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="34"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="12"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" location="Contents!A1" display="Contents!A1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2439,7 +2555,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -2559,11 +2675,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2611,6 +2729,81 @@
         <v>292</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>342</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="Contents!A1" display="Contents!A1"/>
@@ -2619,7 +2812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -2731,7 +2924,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
@@ -3105,7 +3298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -4093,16 +4286,16 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="75" t="s">
         <v>307</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="E3" s="71" t="s">
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="E3" s="75" t="s">
         <v>308</v>
       </c>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -4321,10 +4514,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J63"/>
+  <dimension ref="B2:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4333,20 +4526,20 @@
     <col min="5" max="5" width="3.7109375" customWidth="1"/>
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.85546875" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="75" t="s">
+        <v>319</v>
+      </c>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="H2" s="75" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="H2" s="71" t="s">
-        <v>321</v>
-      </c>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
@@ -4370,7 +4563,7 @@
       <c r="D5" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="F5" s="72"/>
+      <c r="F5" s="71"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
@@ -4416,7 +4609,7 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4440,7 +4633,7 @@
         <v>119</v>
       </c>
       <c r="H13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -4490,7 +4683,7 @@
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H19" s="79" t="s">
+      <c r="H19" s="72" t="s">
         <v>316</v>
       </c>
       <c r="I19" s="10" t="s">
@@ -4509,12 +4702,12 @@
         <v>315</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H21" s="73" t="s">
-        <v>317</v>
-      </c>
-      <c r="I21" s="74"/>
-      <c r="J21" s="75"/>
+    <row r="21" spans="2:10" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="76" t="s">
+        <v>334</v>
+      </c>
+      <c r="I21" s="77"/>
+      <c r="J21" s="78"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="27" t="s">
@@ -4524,9 +4717,9 @@
         <v>106</v>
       </c>
       <c r="D22" s="29"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="77"/>
-      <c r="J22" s="78"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="81"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="30">
@@ -4536,7 +4729,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -4551,325 +4744,359 @@
       </c>
     </row>
     <row r="25" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="80" t="s">
+      <c r="B25" s="73" t="s">
         <v>174</v>
       </c>
       <c r="C25" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="81" t="s">
-        <v>319</v>
+      <c r="D25" s="74" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H30" s="27" t="s">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H30" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="I30" s="28" t="s">
+      <c r="I30" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="J30" s="29"/>
+      <c r="J30" s="21" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="27" t="s">
+      <c r="H31" s="22">
+        <v>4</v>
+      </c>
+      <c r="I31" s="18">
+        <v>2</v>
+      </c>
+      <c r="J31" s="23" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H32" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="I32" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="J32" s="26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H46" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="I46" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D31" s="29"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="32"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="30">
+      <c r="J46" s="29"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" s="29"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="32"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="30">
         <v>4</v>
       </c>
-      <c r="C32" s="31">
+      <c r="C48" s="31">
         <v>2</v>
       </c>
-      <c r="D32" s="32" t="s">
+      <c r="D48" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="H32" s="30"/>
-      <c r="I32" s="31">
+      <c r="H48" s="30"/>
+      <c r="I48" s="31">
         <v>6</v>
       </c>
-      <c r="J32" s="32" t="s">
+      <c r="J48" s="32" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="33" t="s">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C49" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="32" t="s">
+      <c r="D49" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="H33" s="30"/>
-      <c r="I33" s="31" t="s">
+      <c r="H49" s="30"/>
+      <c r="I49" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="J33" s="32" t="s">
+      <c r="J49" s="32" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="30" t="s">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="C34" s="31" t="s">
+      <c r="C50" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="32" t="s">
+      <c r="D50" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="H34" s="30"/>
-      <c r="I34" s="31" t="s">
+      <c r="H50" s="30"/>
+      <c r="I50" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="J34" s="32" t="s">
+      <c r="J50" s="32" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="30" t="s">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="C35" s="31" t="s">
+      <c r="C51" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="32" t="s">
+      <c r="D51" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="H35" s="30"/>
-      <c r="I35" s="31" t="s">
+      <c r="H51" s="30"/>
+      <c r="I51" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="J35" s="32" t="s">
+      <c r="J51" s="32" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="30"/>
-      <c r="C36" s="31" t="s">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="30"/>
+      <c r="C52" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="D36" s="32" t="s">
+      <c r="D52" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="H36" s="30"/>
-      <c r="I36" s="10" t="s">
+      <c r="H52" s="30"/>
+      <c r="I52" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="J36" s="37" t="s">
+      <c r="J52" s="37" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="30" t="s">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C53" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D37" s="32" t="s">
+      <c r="D53" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="H37" s="30"/>
-      <c r="I37" s="31" t="s">
+      <c r="H53" s="30"/>
+      <c r="I53" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="J37" s="37" t="s">
+      <c r="J53" s="37" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="34" t="s">
+    <row r="54" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="34" t="s">
         <v>173</v>
       </c>
-      <c r="C38" s="35" t="s">
+      <c r="C54" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="D38" s="36" t="s">
+      <c r="D54" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="H38" s="30"/>
-      <c r="I38" s="31" t="s">
+      <c r="H54" s="30"/>
+      <c r="I54" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="J38" s="32" t="s">
+      <c r="J54" s="32" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H39" s="30"/>
-      <c r="I39" s="31" t="s">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H55" s="30"/>
+      <c r="I55" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="J39" s="32" t="s">
+      <c r="J55" s="32" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H40" s="30" t="s">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H56" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="I40" s="31" t="s">
+      <c r="I56" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="J40" s="37" t="s">
+      <c r="J56" s="37" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H41" s="30"/>
-      <c r="I41" s="31" t="s">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H57" s="30"/>
+      <c r="I57" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="J41" s="32" t="s">
+      <c r="J57" s="32" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H42" s="34"/>
-      <c r="I42" s="35" t="s">
+    <row r="58" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H58" s="34"/>
+      <c r="I58" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="J42" s="36" t="s">
+      <c r="J58" s="36" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="27" t="s">
+    <row r="61" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B62" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="C46" s="28" t="s">
+      <c r="C62" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D46" s="29"/>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="30">
+      <c r="D62" s="29"/>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B63" s="30">
         <v>4</v>
       </c>
-      <c r="C47" s="31">
+      <c r="C63" s="31">
         <v>5</v>
       </c>
-      <c r="D47" s="37" t="s">
+      <c r="D63" s="37" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="33"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="32" t="s">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B64" s="33"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="32" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="30"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="32" t="s">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="30"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="32" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="30"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="32" t="s">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="30"/>
+      <c r="C66" s="31"/>
+      <c r="D66" s="32" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="30"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="32" t="s">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="30"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="32" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="30"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="37" t="s">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="30"/>
+      <c r="C68" s="31"/>
+      <c r="D68" s="37" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="38"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="32" t="s">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="38"/>
+      <c r="C69" s="31"/>
+      <c r="D69" s="32" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="30"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="37" t="s">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="30"/>
+      <c r="C70" s="31"/>
+      <c r="D70" s="37" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="30"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="37" t="s">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="30"/>
+      <c r="C71" s="31"/>
+      <c r="D71" s="37" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="30"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="37" t="s">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="30"/>
+      <c r="C72" s="31"/>
+      <c r="D72" s="37" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="30"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="37" t="s">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="30"/>
+      <c r="C73" s="31"/>
+      <c r="D73" s="37" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="30"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="32"/>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="30"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="32"/>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="30"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="32"/>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="30"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="32"/>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="30"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="32"/>
-    </row>
-    <row r="63" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="34"/>
-      <c r="C63" s="35"/>
-      <c r="D63" s="36"/>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="30"/>
+      <c r="C74" s="31"/>
+      <c r="D74" s="32"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="30"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="32"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="30"/>
+      <c r="C76" s="31"/>
+      <c r="D76" s="32"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="30"/>
+      <c r="C77" s="31"/>
+      <c r="D77" s="32"/>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="30"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="32"/>
+    </row>
+    <row r="79" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="34"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4890,7 +5117,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
error code array instead one value
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec.xlsx
+++ b/1-SystemDocs/System_spec.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="4" activeTab="12"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="13" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="358">
   <si>
     <t>ETH*</t>
   </si>
@@ -1129,6 +1129,12 @@
   </si>
   <si>
     <t>add error code array instead of one value</t>
+  </si>
+  <si>
+    <t>LED changed to header</t>
+  </si>
+  <si>
+    <t>debug error code sending from multiple units</t>
   </si>
 </sst>
 </file>
@@ -2716,10 +2722,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2920,17 +2926,33 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>352</v>
+        <v>356</v>
+      </c>
+      <c r="B27" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>355</v>
+      </c>
+      <c r="B32" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
error report fixed and sw reset done
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec.xlsx
+++ b/1-SystemDocs/System_spec.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="359">
   <si>
     <t>ETH*</t>
   </si>
@@ -1083,9 +1083,6 @@
     <t>change pca9555 so also the other one can be used</t>
   </si>
   <si>
-    <t>C16 change to 10u, avoid loading fw problems</t>
-  </si>
-  <si>
     <t>SMPS  inductors  to SRP5030CA-1R5M</t>
   </si>
   <si>
@@ -1135,6 +1132,12 @@
   </si>
   <si>
     <t>debug error code sending from multiple units</t>
+  </si>
+  <si>
+    <t>C16 change to 100n, avoid loading fw problems</t>
+  </si>
+  <si>
+    <t>10u tested, works but 100n better for CP2102</t>
   </si>
 </sst>
 </file>
@@ -1696,7 +1699,7 @@
         <xdr:cNvPr id="2" name="Obrázok 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2725,7 +2728,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2764,7 +2767,7 @@
         <v>282</v>
       </c>
       <c r="B5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2772,7 +2775,7 @@
         <v>283</v>
       </c>
       <c r="B6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2782,7 +2785,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2790,7 +2793,7 @@
         <v>326</v>
       </c>
       <c r="B10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2798,7 +2801,7 @@
         <v>327</v>
       </c>
       <c r="B11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2806,7 +2809,7 @@
         <v>328</v>
       </c>
       <c r="B12" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2814,7 +2817,7 @@
         <v>329</v>
       </c>
       <c r="B13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2822,7 +2825,7 @@
         <v>330</v>
       </c>
       <c r="B14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2830,7 +2833,7 @@
         <v>331</v>
       </c>
       <c r="B15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2838,7 +2841,7 @@
         <v>332</v>
       </c>
       <c r="B16" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2846,7 +2849,7 @@
         <v>334</v>
       </c>
       <c r="B17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2854,7 +2857,7 @@
         <v>335</v>
       </c>
       <c r="B18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2862,7 +2865,7 @@
         <v>336</v>
       </c>
       <c r="B19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2870,7 +2873,7 @@
         <v>337</v>
       </c>
       <c r="B20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2878,7 +2881,7 @@
         <v>338</v>
       </c>
       <c r="B21" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2886,73 +2889,76 @@
         <v>339</v>
       </c>
       <c r="B22" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="B23" t="s">
-        <v>347</v>
+        <v>346</v>
+      </c>
+      <c r="C23" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>341</v>
+      </c>
+      <c r="B25" t="s">
+        <v>346</v>
+      </c>
+      <c r="C25" s="57" t="s">
         <v>342</v>
-      </c>
-      <c r="B25" t="s">
-        <v>347</v>
-      </c>
-      <c r="C25" s="57" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B26" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B32" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -5348,7 +5354,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>298</v>
@@ -5394,7 +5400,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed network, ADC begin
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec.xlsx
+++ b/1-SystemDocs/System_spec.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="13" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="363">
   <si>
     <t>ETH*</t>
   </si>
@@ -1138,6 +1138,18 @@
   </si>
   <si>
     <t>10u tested, works but 100n better for CP2102</t>
+  </si>
+  <si>
+    <t>reset was not performed properly, software reset was not wquivalent to HW reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">power report not received from 24 </t>
+  </si>
+  <si>
+    <t>(udp) &amp;&amp; ((udp.dstport == 1111)||(udp.dstport == 1100)||(udp.dstport == 1024)||(udp.dstport == 65500)||(udp.dstport == 65511))</t>
+  </si>
+  <si>
+    <t>Wireshark Filter</t>
   </si>
 </sst>
 </file>
@@ -1699,7 +1711,7 @@
         <xdr:cNvPr id="2" name="Obrázok 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2440,7 +2452,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2725,10 +2737,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2956,9 +2968,20 @@
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>356</v>
+      </c>
+      <c r="B33" t="s">
+        <v>346</v>
+      </c>
+      <c r="C33" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -4358,10 +4381,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4411,6 +4434,16 @@
       </c>
       <c r="C4" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sch main final touches
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec.xlsx
+++ b/1-SystemDocs/System_spec.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="13" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="379">
   <si>
     <t>ETH*</t>
   </si>
@@ -468,21 +468,6 @@
     <t>Retrieve One measurement</t>
   </si>
   <si>
-    <t>Sensor 1</t>
-  </si>
-  <si>
-    <t>Sensor 2</t>
-  </si>
-  <si>
-    <t>Sensor 3</t>
-  </si>
-  <si>
-    <t>Sensor 4</t>
-  </si>
-  <si>
-    <t>Sensor 12</t>
-  </si>
-  <si>
     <t>ADS114S08</t>
   </si>
   <si>
@@ -573,18 +558,6 @@
     <t>ANNOUNCEMENT announcing sensor unit is on network</t>
   </si>
   <si>
-    <t>5..8</t>
-  </si>
-  <si>
-    <t>9..12</t>
-  </si>
-  <si>
-    <t>13..17</t>
-  </si>
-  <si>
-    <t>49..52</t>
-  </si>
-  <si>
     <t>6..7</t>
   </si>
   <si>
@@ -1150,6 +1123,81 @@
   </si>
   <si>
     <t>Wireshark Filter</t>
+  </si>
+  <si>
+    <t>Unit resets</t>
+  </si>
+  <si>
+    <t>range A1.0</t>
+  </si>
+  <si>
+    <t>7..8</t>
+  </si>
+  <si>
+    <t>10..11</t>
+  </si>
+  <si>
+    <t>range A3.3</t>
+  </si>
+  <si>
+    <t>data raw A3.3</t>
+  </si>
+  <si>
+    <t>range A1.1</t>
+  </si>
+  <si>
+    <t>data raw A1.2</t>
+  </si>
+  <si>
+    <t>40..41</t>
+  </si>
+  <si>
+    <t>data raw A1.0 MSB:LSB</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>13..14</t>
+  </si>
+  <si>
+    <t>16..17</t>
+  </si>
+  <si>
+    <t>19..20</t>
+  </si>
+  <si>
+    <t>22..23</t>
+  </si>
+  <si>
+    <t>range A1.2</t>
+  </si>
+  <si>
+    <t>data raw A1.2 MSB:LSB</t>
+  </si>
+  <si>
+    <t>range A1.3</t>
+  </si>
+  <si>
+    <t>data raw A1.3</t>
+  </si>
+  <si>
+    <t>range A2.0</t>
+  </si>
+  <si>
+    <t>data raw A2.0 MSB:LSB</t>
+  </si>
+  <si>
+    <t>range A2.1</t>
+  </si>
+  <si>
+    <t>data raw A2.1</t>
   </si>
 </sst>
 </file>
@@ -1992,6 +2040,56 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1733550</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Rovná spojovacia šípka 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3562350" y="6915150"/>
+          <a:ext cx="1295400" cy="28575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2321,72 +2419,72 @@
     </row>
     <row r="2" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="56" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="56" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="56" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="56" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="56" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B7" s="56" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="56" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B9" s="56" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="56" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B11" s="56" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="56" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="56" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="56" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B15" s="56" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="2:2" ht="21" x14ac:dyDescent="0.35">
@@ -2464,7 +2562,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B1" s="58" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2474,7 +2572,7 @@
     </row>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="67" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="D3" s="30"/>
       <c r="E3" s="31"/>
@@ -2485,7 +2583,7 @@
         <v>500</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="D4" s="30"/>
       <c r="E4" s="31"/>
@@ -2525,87 +2623,87 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
@@ -2635,12 +2733,12 @@
         <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2649,12 +2747,12 @@
         <v>284</v>
       </c>
       <c r="I2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -2665,7 +2763,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B4">
         <v>68</v>
@@ -2674,59 +2772,59 @@
         <v>9000</v>
       </c>
       <c r="D4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B9">
         <v>400</v>
       </c>
       <c r="C9" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B10">
         <f>1/(B9)</f>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="C10" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B11">
         <f>B10*16</f>
         <v>0.04</v>
       </c>
       <c r="C11" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B12">
         <f>B11*9</f>
         <v>0.36</v>
       </c>
       <c r="C12" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2750,7 +2848,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="58" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2758,7 +2856,7 @@
         <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2766,7 +2864,7 @@
         <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2776,212 +2874,212 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="B5" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B6" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B10" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B11" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B12" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B13" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B14" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="B15" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="B16" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B17" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="B18" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B19" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>328</v>
+      </c>
+      <c r="B20" t="s">
         <v>337</v>
-      </c>
-      <c r="B20" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B21" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="B22" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="B23" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="C23" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="B24" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="B25" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="C25" s="57" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B26" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B27" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="B32" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="B33" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="C33" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -3011,7 +3109,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3019,7 +3117,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3027,7 +3125,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3035,7 +3133,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3043,7 +3141,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3051,7 +3149,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3059,7 +3157,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3067,7 +3165,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3126,42 +3224,42 @@
   <sheetData>
     <row r="1" spans="1:13" s="59" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="58" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" t="s">
+        <v>202</v>
+      </c>
+      <c r="I2" t="s">
+        <v>203</v>
+      </c>
+      <c r="J2" t="s">
+        <v>204</v>
+      </c>
+      <c r="K2" t="s">
+        <v>261</v>
+      </c>
+      <c r="L2" t="s">
         <v>208</v>
       </c>
-      <c r="D2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E2" t="s">
-        <v>221</v>
-      </c>
-      <c r="F2" t="s">
-        <v>210</v>
-      </c>
-      <c r="G2" t="s">
-        <v>209</v>
-      </c>
-      <c r="H2" t="s">
-        <v>211</v>
-      </c>
-      <c r="I2" t="s">
-        <v>212</v>
-      </c>
-      <c r="J2" t="s">
-        <v>213</v>
-      </c>
-      <c r="K2" t="s">
-        <v>270</v>
-      </c>
-      <c r="L2" t="s">
-        <v>217</v>
-      </c>
       <c r="M2" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3169,34 +3267,34 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="D3" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="E3" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="F3">
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="H3" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="I3" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="J3" s="60" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="K3" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="L3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -3204,28 +3302,28 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D4" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="F4" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="H4" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="I4" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="J4" s="61" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="K4" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="L4" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3233,31 +3331,31 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D5" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="E5" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="G5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="H5" t="s">
+        <v>216</v>
+      </c>
+      <c r="I5" t="s">
+        <v>220</v>
+      </c>
+      <c r="J5" s="62" t="s">
+        <v>223</v>
+      </c>
+      <c r="K5" t="s">
+        <v>264</v>
+      </c>
+      <c r="M5" s="57" t="s">
         <v>225</v>
-      </c>
-      <c r="I5" t="s">
-        <v>229</v>
-      </c>
-      <c r="J5" s="62" t="s">
-        <v>232</v>
-      </c>
-      <c r="K5" t="s">
-        <v>273</v>
-      </c>
-      <c r="M5" s="57" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -3265,25 +3363,25 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D6" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="F6" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="H6" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="I6" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="J6" s="61" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="K6" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3291,25 +3389,25 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D7" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="F7" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="H7" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="I7" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="J7" s="61" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="K7" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -3317,19 +3415,19 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D8" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="H8" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="I8" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="J8" s="61" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -3337,28 +3435,28 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="D9" t="s">
+        <v>239</v>
+      </c>
+      <c r="F9" t="s">
+        <v>241</v>
+      </c>
+      <c r="G9" t="s">
+        <v>242</v>
+      </c>
+      <c r="H9" t="s">
         <v>248</v>
       </c>
-      <c r="F9" t="s">
-        <v>250</v>
-      </c>
-      <c r="G9" t="s">
-        <v>251</v>
-      </c>
-      <c r="H9" t="s">
-        <v>257</v>
-      </c>
       <c r="I9" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="J9" s="64" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="L9" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -3366,25 +3464,25 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="D10" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="F10" t="s">
         <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="H10" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="I10" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="J10" s="64" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -3392,19 +3490,19 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D11" t="s">
+        <v>251</v>
+      </c>
+      <c r="H11" t="s">
+        <v>252</v>
+      </c>
+      <c r="I11" t="s">
         <v>258</v>
       </c>
-      <c r="D11" t="s">
-        <v>260</v>
-      </c>
-      <c r="H11" t="s">
-        <v>261</v>
-      </c>
-      <c r="I11" t="s">
-        <v>267</v>
-      </c>
       <c r="J11" s="63" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -3412,22 +3510,22 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="D12" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="F12" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="H12" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="I12" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="J12" s="65" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -3435,10 +3533,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="J13" s="64" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -3446,13 +3544,13 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="H14" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="J14" s="66" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -3492,20 +3590,20 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="58" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B4" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -3535,7 +3633,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
@@ -3559,7 +3657,7 @@
         <v>74</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -3642,7 +3740,7 @@
         <v>44</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="L4" s="1">
         <v>4</v>
@@ -3671,10 +3769,10 @@
         <v>12</v>
       </c>
       <c r="J5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="L5" s="1">
         <v>17</v>
@@ -3703,7 +3801,7 @@
         <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>14</v>
@@ -3776,7 +3874,7 @@
         <v>23</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="L9" s="1">
         <v>23</v>
@@ -4383,7 +4481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -4438,12 +4536,12 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -4457,7 +4555,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:G3"/>
+      <selection activeCell="B20" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4478,12 +4576,12 @@
     </row>
     <row r="3" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="75" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B3" s="75"/>
       <c r="C3" s="75"/>
       <c r="E3" s="75" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="F3" s="75"/>
       <c r="G3" s="75"/>
@@ -4513,7 +4611,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>103</v>
@@ -4522,7 +4620,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>103</v>
@@ -4533,7 +4631,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>103</v>
@@ -4542,7 +4640,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>103</v>
@@ -4553,7 +4651,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>103</v>
@@ -4562,7 +4660,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>103</v>
@@ -4573,7 +4671,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>103</v>
@@ -4582,7 +4680,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>103</v>
@@ -4613,19 +4711,19 @@
         <v>5</v>
       </c>
       <c r="B10" s="69" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="C10" s="69" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="E10" s="69">
         <v>5</v>
       </c>
       <c r="F10" s="69" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="G10" s="69" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4705,10 +4803,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J79"/>
+  <dimension ref="B2:L79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:C23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4722,12 +4820,12 @@
   <sheetData>
     <row r="2" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="75" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="C2" s="75"/>
       <c r="D2" s="75"/>
       <c r="H2" s="75" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="I2" s="75"/>
       <c r="J2" s="75"/>
@@ -4752,7 +4850,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="55" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F5" s="71"/>
     </row>
@@ -4800,7 +4898,7 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4824,7 +4922,7 @@
         <v>119</v>
       </c>
       <c r="H13" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -4835,7 +4933,7 @@
         <v>101</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4870,32 +4968,32 @@
         <v>5</v>
       </c>
       <c r="J18" s="37" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H19" s="72" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="J19" s="37" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H20" s="30"/>
       <c r="I20" s="10" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="J20" s="37" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H21" s="76" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="I21" s="77"/>
       <c r="J21" s="78"/>
@@ -4920,7 +5018,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -4931,23 +5029,23 @@
         <v>101</v>
       </c>
       <c r="D24" s="37" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="73" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C25" s="35" t="s">
         <v>99</v>
       </c>
       <c r="D25" s="74" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4963,6 +5061,9 @@
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>354</v>
+      </c>
       <c r="H31" s="22">
         <v>4</v>
       </c>
@@ -4970,7 +5071,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4984,8 +5085,148 @@
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="29"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="30">
+        <v>4</v>
+      </c>
+      <c r="C36" s="31">
+        <v>2</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="30">
+        <v>5</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="K37" t="s">
+        <v>364</v>
+      </c>
+      <c r="L37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="30">
+        <v>6</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>355</v>
+      </c>
+      <c r="K38" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="30" t="s">
+        <v>356</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>363</v>
+      </c>
+      <c r="K39" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="30">
+        <v>9</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="30" t="s">
+        <v>357</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="30">
+        <v>12</v>
+      </c>
+      <c r="C42" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="30" t="s">
+        <v>367</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="30">
+        <v>15</v>
+      </c>
+      <c r="C44" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="30" t="s">
+        <v>368</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" s="32" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="30">
+        <v>18</v>
+      </c>
+      <c r="C46" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>375</v>
+      </c>
       <c r="H46" s="27" t="s">
         <v>105</v>
       </c>
@@ -4994,27 +5235,29 @@
       </c>
       <c r="J46" s="29"/>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="C47" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D47" s="29"/>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="30" t="s">
+        <v>369</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="32" t="s">
+        <v>376</v>
+      </c>
       <c r="H47" s="30"/>
       <c r="I47" s="31"/>
       <c r="J47" s="32"/>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" s="30">
-        <v>4</v>
-      </c>
-      <c r="C48" s="31">
-        <v>2</v>
+        <v>21</v>
+      </c>
+      <c r="C48" s="31" t="s">
+        <v>101</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>104</v>
+        <v>377</v>
       </c>
       <c r="H48" s="30"/>
       <c r="I48" s="31">
@@ -5025,14 +5268,14 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="33" t="s">
-        <v>170</v>
+      <c r="B49" s="30" t="s">
+        <v>370</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>135</v>
+        <v>378</v>
       </c>
       <c r="H49" s="30"/>
       <c r="I49" s="31" t="s">
@@ -5044,13 +5287,13 @@
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="30" t="s">
-        <v>171</v>
+        <v>129</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="H50" s="30"/>
       <c r="I50" s="31" t="s">
@@ -5061,14 +5304,14 @@
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="30" t="s">
-        <v>172</v>
+      <c r="B51" s="30">
+        <v>39</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>137</v>
+        <v>358</v>
       </c>
       <c r="H51" s="30"/>
       <c r="I51" s="31" t="s">
@@ -5078,13 +5321,15 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="30"/>
-      <c r="C52" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="D52" s="32" t="s">
-        <v>138</v>
+    <row r="52" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="34" t="s">
+        <v>362</v>
+      </c>
+      <c r="C52" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52" s="36" t="s">
+        <v>359</v>
       </c>
       <c r="H52" s="30"/>
       <c r="I52" s="10" t="s">
@@ -5095,15 +5340,6 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="D53" s="32" t="s">
-        <v>129</v>
-      </c>
       <c r="H53" s="30"/>
       <c r="I53" s="31" t="s">
         <v>133</v>
@@ -5112,16 +5348,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="34" t="s">
-        <v>173</v>
-      </c>
-      <c r="C54" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="D54" s="36" t="s">
-        <v>139</v>
-      </c>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H54" s="30"/>
       <c r="I54" s="31" t="s">
         <v>101</v>
@@ -5186,7 +5413,10 @@
         <v>5</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>301</v>
+        <v>292</v>
+      </c>
+      <c r="E63" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -5249,14 +5479,14 @@
       <c r="B72" s="30"/>
       <c r="C72" s="31"/>
       <c r="D72" s="37" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="30"/>
       <c r="C73" s="31"/>
       <c r="D73" s="37" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
@@ -5320,7 +5550,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B1" s="58" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -5334,7 +5564,7 @@
     </row>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="67" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="D3" s="30">
         <v>4</v>
@@ -5351,7 +5581,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="D4" s="30">
         <v>5</v>
@@ -5368,7 +5598,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="35"/>
@@ -5379,7 +5609,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -5387,10 +5617,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -5398,10 +5628,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="D8" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -5409,7 +5639,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -5417,7 +5647,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -5425,7 +5655,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -5433,7 +5663,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>